<commit_message>
add full file path to data sheet
</commit_message>
<xml_diff>
--- a/spry-1620/datasheet.xlsx
+++ b/spry-1620/datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timbarry/research_code/GENETHOFF/spry-1620/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F150D1FD-8BD4-494A-9C1A-E45FB125FCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB16767E-6C65-DC47-BA00-811E9695D849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2140" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{A849A2B9-5AEE-407F-80B9-CAB473E64C7A}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>TAGCCATG</t>
   </si>
   <si>
-    <t>$HOME/research_offsite/external/bauer-lab/guideseq/fastq_files</t>
-  </si>
-  <si>
     <t>293T_SpRY_Cas9_1620_GSPneg_S79_S87</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>grna_1620</t>
+  </si>
+  <si>
+    <t>/home/tib163/research_offsite/external/bauer-lab/guideseq/fastq_files</t>
   </si>
 </sst>
 </file>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4ACCEC-A3C9-495B-9DB4-02B207EEC8AA}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -581,7 +581,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -590,7 +590,7 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -620,12 +620,12 @@
         <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -634,7 +634,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -658,18 +658,18 @@
         <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M3" t="s">
         <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -678,7 +678,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -702,18 +702,18 @@
         <v>15</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M4" t="s">
         <v>23</v>
       </c>
       <c r="N4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -722,7 +722,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -746,13 +746,13 @@
         <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M5" t="s">
         <v>23</v>
       </c>
       <c r="N5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>